<commit_message>
Updated PCA table, with treatments column added
</commit_message>
<xml_diff>
--- a/data/ofv_pca_table.xlsx
+++ b/data/ofv_pca_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH28"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,165 +365,170 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Toulene</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Hexanal &lt;n-&gt;</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Xylene &lt;m-&gt;</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Oxime, methoxy-phenyl-</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Pinene &lt;1R-alpha-&gt;</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Carene, &lt;3-&gt;</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Phellandrene &lt;beta-&gt;</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Pinene &lt;beta-&gt;</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Mesitylene</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>p-Cymene</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>D-Limonene</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Pinene &lt;alpha-&gt;</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Carene &lt;delta-3&gt;</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Dodecane</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Undecane</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Nonanal</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Limonene oxide, trans-</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Benzaldehyde &lt;para-ethyl-&gt;</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>1-Nonanol</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Terpineol &lt;alpha-&gt;</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Decanal</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Pentadecane</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>2-cyclopentylcyclopentan-1-one</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Copaene &lt;alpha-&gt;</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Bourbonene &lt;beta-&gt;</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Caryophyllene</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Cubebene &lt;beta-&gt;</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Bergamotene &lt;alpha-, cis-&gt;</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Zonarene</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Murrolene &lt;gamma-&gt;</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Murrolene &lt;alpha-&gt;</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Farnesene &lt;(E,E)-, alpha-&gt;</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Caryophyllene oxide</t>
         </is>
@@ -535,8 +540,10 @@
           <t>rose_1ul_nonyl_acetate</t>
         </is>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C2">
         <v>0</v>
@@ -551,50 +558,50 @@
         <v>0</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>0.002944496248946039</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2.127506212263892e-005</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.001652110154514978</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>0.0002493834961389282</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>3.34266359271267e-005</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>9.691103293237313e-005</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
       <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>9.784985153719247e-006</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>1.275923067984926e-005</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>0.005635397815953328</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
       <c r="V2">
         <v>0</v>
       </c>
@@ -602,36 +609,39 @@
         <v>0</v>
       </c>
       <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
         <v>0.001776939545321152</v>
       </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
         <v>0.01782273743793637</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>0.0009164048528676767</v>
       </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
       <c r="AD2">
         <v>0</v>
       </c>
       <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
         <v>0.05304955311074119</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>0.001691896454062633</v>
       </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
       <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
         <v>0</v>
       </c>
     </row>
@@ -641,33 +651,35 @@
           <t>rose_clean_actigard_site_1</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>actigard</t>
+        </is>
+      </c>
+      <c r="C3">
         <v>0.178558508427826</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>5.855463345427039</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0.0753423220516936</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0.02562503824823455</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
@@ -708,11 +720,11 @@
         <v>0</v>
       </c>
       <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
         <v>0.1609951251131896</v>
       </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
       <c r="Z3">
         <v>0</v>
       </c>
@@ -738,6 +750,9 @@
         <v>0</v>
       </c>
       <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
         <v>0</v>
       </c>
     </row>
@@ -747,8 +762,10 @@
           <t>rose_clean_actigard_site_2</t>
         </is>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>actigard</t>
+        </is>
       </c>
       <c r="C4">
         <v>0</v>
@@ -757,23 +774,23 @@
         <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0.2269229083095019</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
       <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.004133005733119027</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>0.0005168282726252787</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
@@ -802,11 +819,11 @@
         <v>0</v>
       </c>
       <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>0.03160346281142813</v>
       </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
       <c r="V4">
         <v>0</v>
       </c>
@@ -814,11 +831,11 @@
         <v>0</v>
       </c>
       <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
         <v>0.007570145060804571</v>
       </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
       <c r="Z4">
         <v>0</v>
       </c>
@@ -835,15 +852,18 @@
         <v>0</v>
       </c>
       <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <v>0.00305461537712743</v>
       </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
       <c r="AG4">
         <v>0</v>
       </c>
       <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
         <v>0</v>
       </c>
     </row>
@@ -853,8 +873,10 @@
           <t>rose_clean_actigard_site_3</t>
         </is>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>actigard</t>
+        </is>
       </c>
       <c r="C5">
         <v>0</v>
@@ -863,23 +885,23 @@
         <v>0</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1.463289029790596</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.02160639953133457</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0.0003561004269297467</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.001904844227486562</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
@@ -908,17 +930,17 @@
         <v>0</v>
       </c>
       <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>0.0183289130230575</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
       <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>0.01285226300634206</v>
       </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
       <c r="X5">
         <v>0</v>
       </c>
@@ -950,6 +972,9 @@
         <v>0</v>
       </c>
       <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>0</v>
       </c>
     </row>
@@ -959,8 +984,10 @@
           <t>rose_clean_actigard_site_4</t>
         </is>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>actigard</t>
+        </is>
       </c>
       <c r="C6">
         <v>0</v>
@@ -969,23 +996,23 @@
         <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0.1143363639569969</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>0.0003744529029109473</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0.0001192305773524972</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
@@ -1056,6 +1083,9 @@
         <v>0</v>
       </c>
       <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
         <v>0</v>
       </c>
     </row>
@@ -1065,8 +1095,10 @@
           <t>rose_clean_actigard_site_5</t>
         </is>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>actigard</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1075,23 +1107,23 @@
         <v>0</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>0.1285944053683378</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0.0004335576982642197</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>3.303943536679731e-005</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.0001673510157667927</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
@@ -1120,11 +1152,11 @@
         <v>0</v>
       </c>
       <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <v>0.03796292823608351</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
       <c r="V7">
         <v>0</v>
       </c>
@@ -1132,11 +1164,11 @@
         <v>0</v>
       </c>
       <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
         <v>0.01085746668480129</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
       <c r="Z7">
         <v>0</v>
       </c>
@@ -1153,15 +1185,18 @@
         <v>0</v>
       </c>
       <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
         <v>0.005167187676674168</v>
       </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
       <c r="AG7">
         <v>0</v>
       </c>
       <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
         <v>0</v>
       </c>
     </row>
@@ -1171,8 +1206,10 @@
           <t>rose_clean_site_11</t>
         </is>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1181,23 +1218,23 @@
         <v>0</v>
       </c>
       <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>0.4749968490740416</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.0598465896785001</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>0.0006816046382966921</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.02724387239224407</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
@@ -1211,47 +1248,47 @@
         <v>0</v>
       </c>
       <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>0.01904730809727568</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.002355823275741833</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.01090503643717584</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <v>0.149880520813224</v>
       </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
       <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>0.006890378356375152</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0.01561994422801373</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>0.01622810050787019</v>
       </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
       <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
         <v>0.003386818443980787</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>0.001768981301625935</v>
       </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
       <c r="AC8">
         <v>0</v>
       </c>
@@ -1259,15 +1296,18 @@
         <v>0</v>
       </c>
       <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
         <v>0.1028537661896217</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>0.005245904372095588</v>
       </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
       <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <v>0</v>
       </c>
     </row>
@@ -1277,72 +1317,74 @@
           <t>rose_clean_site_12</t>
         </is>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>0.09215725150776628</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.5505406638993413</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.002680839127803835</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>9.653474020083978e-005</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.0005152469584579358</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
         <v>0.23097687880581</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
       <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>8.051028413673042e-005</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>0.03246391053472224</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>0.0001056190245357149</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <v>0.1006570590279598</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>0.0001172956504692572</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>0.005183494938264659</v>
       </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
       <c r="X9">
         <v>0</v>
       </c>
@@ -1374,6 +1416,9 @@
         <v>0</v>
       </c>
       <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <v>0</v>
       </c>
     </row>
@@ -1383,42 +1428,44 @@
           <t>rose_clean_site_13</t>
         </is>
       </c>
-      <c r="B10">
-        <v>0</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>0.0297360307156277</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.4146550365085263</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
       <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0.03203723329332277</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.0001696681704685768</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.02084790510555729</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <v>0.08001849615655626</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
       <c r="N10">
         <v>0</v>
       </c>
@@ -1438,23 +1485,23 @@
         <v>0</v>
       </c>
       <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <v>0.07710118739776441</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
       <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>0.001775406358881487</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>0.002473950552121455</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>0.003670760843591019</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
       <c r="Z10">
         <v>0</v>
       </c>
@@ -1471,15 +1518,18 @@
         <v>0</v>
       </c>
       <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
         <v>0.05713784935834351</v>
       </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
       <c r="AG10">
         <v>0</v>
       </c>
       <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
         <v>0</v>
       </c>
     </row>
@@ -1489,21 +1539,23 @@
           <t>rose_clean_site_14</t>
         </is>
       </c>
-      <c r="B11">
-        <v>0</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>0.002559216729294696</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.008429317785955447</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
       <c r="G11">
         <v>0</v>
       </c>
@@ -1520,20 +1572,20 @@
         <v>0</v>
       </c>
       <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
         <v>0.002357116793804675</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>0.0005554502480222632</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
       <c r="Q11">
         <v>0</v>
       </c>
@@ -1541,20 +1593,20 @@
         <v>0</v>
       </c>
       <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>1.42707138232056e-005</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>0.08627946517597344</v>
       </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
       <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
         <v>0.0003924977740774261</v>
       </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
       <c r="X11">
         <v>0</v>
       </c>
@@ -1577,15 +1629,18 @@
         <v>0</v>
       </c>
       <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
         <v>0.004353975778086736</v>
       </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
       <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
         <v>1.500180138027962e-005</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>0</v>
       </c>
     </row>
@@ -1595,42 +1650,44 @@
           <t>rose_clean_site_15</t>
         </is>
       </c>
-      <c r="B12">
-        <v>0</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>0.4662810796563268</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2.327862175161385</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
       <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>0.1276065089936959</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.001236685065466652</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.09498324835535868</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>0.6731412760099993</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
       <c r="N12">
         <v>0</v>
       </c>
@@ -1650,48 +1707,51 @@
         <v>0</v>
       </c>
       <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
         <v>0.02721577020755985</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
       <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <v>0.04798385806722944</v>
       </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
       <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <v>0.03780009752520438</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>0.0004980678220398041</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
       <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
         <v>0.01809629389519563</v>
       </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
       <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
         <v>0.0005034651699772933</v>
       </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
       <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
         <v>0.4320225170177273</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>0.01950005462051566</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>0.000751925596105495</v>
       </c>
-      <c r="AH12">
+      <c r="AI12">
         <v>0</v>
       </c>
     </row>
@@ -1701,42 +1761,44 @@
           <t>rose_clean_site_16</t>
         </is>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>0.1115899811688947</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>0.7436399030627555</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>0.02169570579187173</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.000199374616995231</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.0159513675104636</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>0.1872862874255729</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
       <c r="N13">
         <v>0</v>
       </c>
@@ -1756,23 +1818,23 @@
         <v>0</v>
       </c>
       <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
         <v>0.1156153637445746</v>
       </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
       <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>0.01063718545552727</v>
       </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
       <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
         <v>0.006322698006665785</v>
       </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
       <c r="Z13">
         <v>0</v>
       </c>
@@ -1789,15 +1851,18 @@
         <v>0</v>
       </c>
       <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <v>0.04426432267371663</v>
       </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
       <c r="AG13">
         <v>0</v>
       </c>
       <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
         <v>0</v>
       </c>
     </row>
@@ -1807,42 +1872,44 @@
           <t>rose_clean_site_17</t>
         </is>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>0.2488475542405619</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2.183278170538528</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
       <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>0.0671607318341433</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.0005251248087339011</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.04367141130847899</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>0.4538107383275493</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
       <c r="N14">
         <v>0</v>
       </c>
@@ -1862,48 +1929,51 @@
         <v>0</v>
       </c>
       <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
         <v>0.144500692419121</v>
       </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
       <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
         <v>0.01740347872348829</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>0.01095086273765797</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>0.02642530642083634</v>
       </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
       <c r="Z14">
         <v>0</v>
       </c>
       <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
         <v>0.0004506671887154416</v>
       </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
       <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
         <v>0.0003362385473378804</v>
       </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
       <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
         <v>0.2279475247834019</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>0.000557079426325299</v>
       </c>
-      <c r="AG14">
-        <v>0</v>
-      </c>
       <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
         <v>0</v>
       </c>
     </row>
@@ -1913,42 +1983,44 @@
           <t>rose_clean_site_18</t>
         </is>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>0.05870768805498415</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.4685037486106246</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>0.02383720711687443</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.0003652103299114953</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.01827254560797554</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>0.130172945968137</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
       <c r="N15">
         <v>0</v>
       </c>
@@ -1968,48 +2040,51 @@
         <v>0</v>
       </c>
       <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
         <v>0.02845216948481091</v>
       </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
       <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
         <v>0.005135891966507977</v>
       </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
       <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
         <v>0.01543022490599929</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>0.0001277159663011801</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
       <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
         <v>0.00425467398330959</v>
       </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
       <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
         <v>0.0001226489442011666</v>
       </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
       <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
         <v>0.04290107497606945</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>8.96850891262226e-005</v>
       </c>
-      <c r="AG15">
-        <v>0</v>
-      </c>
       <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
         <v>0</v>
       </c>
     </row>
@@ -2019,42 +2094,44 @@
           <t>rose_clean_site_19</t>
         </is>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>0.4429687197660229</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>2.445830947639219</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>0.03888475727758896</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.0003334323283649964</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.01789187223662405</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>0.5893162254887632</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
       <c r="N16">
         <v>0</v>
       </c>
@@ -2074,23 +2151,23 @@
         <v>0</v>
       </c>
       <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
         <v>0.07453825965545805</v>
       </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
       <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <v>0.01531805461689526</v>
       </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
       <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
         <v>0.006396408656012634</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
       <c r="Z16">
         <v>0</v>
       </c>
@@ -2107,15 +2184,18 @@
         <v>0</v>
       </c>
       <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
         <v>0.02050890625870869</v>
       </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
       <c r="AG16">
         <v>0</v>
       </c>
       <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
         <v>0</v>
       </c>
     </row>
@@ -2125,42 +2205,44 @@
           <t>rose_clean_site_20</t>
         </is>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>untreated</t>
+        </is>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>0.1763479689222839</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>0.8947744735679123</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>0.05543029208045386</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.0001933422894438156</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.02850906689935885</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>0.2221119890346135</v>
       </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
       <c r="N17">
         <v>0</v>
       </c>
@@ -2180,23 +2262,23 @@
         <v>0</v>
       </c>
       <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
         <v>0.07864270049389376</v>
       </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
       <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
         <v>0.007193953660878046</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
       <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
         <v>0.004715034688379863</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
       <c r="Z17">
         <v>0</v>
       </c>
@@ -2213,15 +2295,18 @@
         <v>0</v>
       </c>
       <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <v>0.04831928334732197</v>
       </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
       <c r="AG17">
         <v>0</v>
       </c>
       <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
         <v>0</v>
       </c>
     </row>
@@ -2231,8 +2316,10 @@
           <t>rose_rrv_site_1-1</t>
         </is>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2241,26 +2328,26 @@
         <v>0</v>
       </c>
       <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>0.6351634859781747</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>0.005773689904659293</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>0.008573719573189672</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
       <c r="L18">
         <v>0</v>
       </c>
@@ -2271,11 +2358,11 @@
         <v>0</v>
       </c>
       <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <v>0.006257274713811328</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
       <c r="Q18">
         <v>0</v>
       </c>
@@ -2286,32 +2373,32 @@
         <v>0</v>
       </c>
       <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <v>0.05387712808730748</v>
       </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
       <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
         <v>0.009123072081142079</v>
       </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
       <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <v>0.01299955002614557</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
       <c r="Z18">
         <v>0</v>
       </c>
       <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
         <v>0.005631244197669024</v>
       </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
       <c r="AC18">
         <v>0</v>
       </c>
@@ -2319,15 +2406,18 @@
         <v>0</v>
       </c>
       <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
         <v>0.02583287012573771</v>
       </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
       <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
         <v>0.0004671178940117932</v>
       </c>
-      <c r="AH18">
+      <c r="AI18">
         <v>0</v>
       </c>
     </row>
@@ -2337,8 +2427,10 @@
           <t>rose_rrv_site_1-2</t>
         </is>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2347,26 +2439,26 @@
         <v>0</v>
       </c>
       <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>0.1193670930208808</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
       <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>0.0007420810464146082</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>0.000121208668676557</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.002855481978234827</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
       <c r="L19">
         <v>0</v>
       </c>
@@ -2374,11 +2466,11 @@
         <v>0</v>
       </c>
       <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>0.0001246257058845803</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
       <c r="P19">
         <v>0</v>
       </c>
@@ -2389,51 +2481,54 @@
         <v>0</v>
       </c>
       <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
         <v>6.129110744785906e-005</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>0.0595643696435374</v>
       </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
       <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
         <v>0.002707561021643164</v>
       </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
       <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
         <v>0.001913159488815808</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>6.423162909224922e-005</v>
       </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
       <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
         <v>0.01298457121706592</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>2.854250392404357e-005</v>
       </c>
-      <c r="AC19">
-        <v>0</v>
-      </c>
       <c r="AD19">
         <v>0</v>
       </c>
       <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
         <v>0.04313807470268002</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>0.001573389087283214</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>4.393202939216404e-005</v>
       </c>
-      <c r="AH19">
+      <c r="AI19">
         <v>3.135088638485835e-005</v>
       </c>
     </row>
@@ -2443,8 +2538,10 @@
           <t>rose_rrv_site_1-3</t>
         </is>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2453,41 +2550,41 @@
         <v>0</v>
       </c>
       <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>0.2591470987242759</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
       <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>0.007451294171326697</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>0.003739120712460542</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.004290575106228864</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <v>0.0001910013605768861</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>0.0004050005812143798</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>0.002538337485990358</v>
       </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
       <c r="Q20">
         <v>0</v>
       </c>
@@ -2498,48 +2595,51 @@
         <v>0</v>
       </c>
       <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
         <v>0.02250248030487999</v>
       </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
       <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
         <v>0.005269070592021741</v>
       </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
       <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
         <v>0.002547580960842977</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>8.026733353729087e-005</v>
       </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
       <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
         <v>0.02476470156976009</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>5.708858560314298e-005</v>
       </c>
-      <c r="AC20">
-        <v>0</v>
-      </c>
       <c r="AD20">
         <v>0</v>
       </c>
       <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
         <v>0.1012071599113805</v>
       </c>
-      <c r="AF20">
+      <c r="AG20">
         <v>0.003393896564329514</v>
       </c>
-      <c r="AG20">
+      <c r="AH20">
         <v>5.91958179028238e-005</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <v>5.461101361702934e-005</v>
       </c>
     </row>
@@ -2549,8 +2649,10 @@
           <t>rose_rrv_site_1-4</t>
         </is>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2559,23 +2661,23 @@
         <v>0</v>
       </c>
       <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>0.2219340736162666</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>0.003442250366024336</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>0.0004637109099481195</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="K21">
         <v>0</v>
       </c>
@@ -2586,11 +2688,11 @@
         <v>0</v>
       </c>
       <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
         <v>0.0002450551560677248</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
       <c r="P21">
         <v>0</v>
       </c>
@@ -2604,32 +2706,32 @@
         <v>0</v>
       </c>
       <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <v>0.0504100079366952</v>
       </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
       <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
         <v>0.006861247689101504</v>
       </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
       <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
         <v>0.003447396947067187</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>0.001428798078299107</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>0.001800535343969719</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <v>0.013378301293068</v>
       </c>
-      <c r="AB21">
-        <v>0</v>
-      </c>
       <c r="AC21">
         <v>0</v>
       </c>
@@ -2637,15 +2739,18 @@
         <v>0</v>
       </c>
       <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
         <v>0.05398698471835284</v>
       </c>
-      <c r="AF21">
-        <v>0</v>
-      </c>
       <c r="AG21">
         <v>0</v>
       </c>
       <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
         <v>0</v>
       </c>
     </row>
@@ -2655,54 +2760,56 @@
           <t>rose_rrv_site_2-1</t>
         </is>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0.03239558202843346</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
       <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>2.613660523435034</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
       <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>0.1540710624145915</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>0.001342782601812019</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>0.1021945747858815</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>0.1492194295318386</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>0.01107962054727577</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
       <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
         <v>0.0175896159601798</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>0.04956042269062311</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>0.01979498833389905</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>0.02739630919343107</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
       <c r="R22">
         <v>0</v>
       </c>
@@ -2716,42 +2823,45 @@
         <v>0</v>
       </c>
       <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
         <v>0.09789249348091567</v>
       </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
       <c r="X22">
         <v>0</v>
       </c>
       <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
         <v>0.0285478170431452</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>0.04843299034577839</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <v>0.670636743112209</v>
       </c>
-      <c r="AB22">
+      <c r="AC22">
         <v>0.04254485115120047</v>
       </c>
-      <c r="AC22">
-        <v>0</v>
-      </c>
       <c r="AD22">
         <v>0</v>
       </c>
       <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
         <v>3.183691563526181</v>
       </c>
-      <c r="AF22">
+      <c r="AG22">
         <v>0.07458370643390686</v>
       </c>
-      <c r="AG22">
+      <c r="AH22">
         <v>0.00565328845370798</v>
       </c>
-      <c r="AH22">
+      <c r="AI22">
         <v>0</v>
       </c>
     </row>
@@ -2761,8 +2871,10 @@
           <t>rose_rrv_site_2-2</t>
         </is>
       </c>
-      <c r="B23">
-        <v>0</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2771,29 +2883,29 @@
         <v>0</v>
       </c>
       <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>0.2782151455941799</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
       <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>0.002189525538460369</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>0.0009089962723814097</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>0.006482894864210993</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>0.01019310748786668</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
       <c r="M23">
         <v>0</v>
       </c>
@@ -2801,11 +2913,11 @@
         <v>0</v>
       </c>
       <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>0.006863569898633267</v>
       </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
       <c r="Q23">
         <v>0</v>
       </c>
@@ -2816,17 +2928,17 @@
         <v>0</v>
       </c>
       <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
         <v>0.06916120993410781</v>
       </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
       <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
         <v>0.008348514734709942</v>
       </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
       <c r="X23">
         <v>0</v>
       </c>
@@ -2849,15 +2961,18 @@
         <v>0</v>
       </c>
       <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
         <v>0.02036841154896054</v>
       </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
       <c r="AG23">
         <v>0</v>
       </c>
       <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
         <v>0</v>
       </c>
     </row>
@@ -2867,8 +2982,10 @@
           <t>rose_rrv_site_2-3</t>
         </is>
       </c>
-      <c r="B24">
-        <v>0</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2877,17 +2994,17 @@
         <v>0</v>
       </c>
       <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>0.3867532227091845</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
       <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>0.001310048812584854</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
       <c r="I24">
         <v>0</v>
       </c>
@@ -2895,23 +3012,23 @@
         <v>0</v>
       </c>
       <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
         <v>0.02744071970110688</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>0.1358041884324002</v>
       </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
         <v>0.003501165111717024</v>
       </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
       <c r="Q24">
         <v>0</v>
       </c>
@@ -2922,17 +3039,17 @@
         <v>0</v>
       </c>
       <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
         <v>0.01666128242249028</v>
       </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
       <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
         <v>0.0077253677498409</v>
       </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
       <c r="X24">
         <v>0</v>
       </c>
@@ -2955,15 +3072,18 @@
         <v>0</v>
       </c>
       <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
         <v>0.008986191728195207</v>
       </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
       <c r="AG24">
         <v>0</v>
       </c>
       <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
         <v>0</v>
       </c>
     </row>
@@ -2973,8 +3093,10 @@
           <t>rose_rrv_site_3-1</t>
         </is>
       </c>
-      <c r="B25">
-        <v>0</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2983,44 +3105,44 @@
         <v>0</v>
       </c>
       <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
         <v>0.9272631485723495</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>0.04640789767597565</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.0006349599627965344</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>0.02973756711197755</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>0.003887814413534992</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
       <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
         <v>0.008446301835707026</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.04008107236507013</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>0.0002785858493154259</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>0.0004786514217163175</v>
       </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
       <c r="R25">
         <v>0</v>
       </c>
@@ -3028,11 +3150,11 @@
         <v>0</v>
       </c>
       <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
         <v>0.06595574270350957</v>
       </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
       <c r="V25">
         <v>0</v>
       </c>
@@ -3043,33 +3165,36 @@
         <v>0</v>
       </c>
       <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <v>0.009432573357695127</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>0.01893953541891401</v>
       </c>
-      <c r="AA25">
+      <c r="AB25">
         <v>0.2325580335475138</v>
       </c>
-      <c r="AB25">
+      <c r="AC25">
         <v>0.01551182597737079</v>
       </c>
-      <c r="AC25">
-        <v>0</v>
-      </c>
       <c r="AD25">
         <v>0</v>
       </c>
       <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
         <v>0.8240605005672281</v>
       </c>
-      <c r="AF25">
+      <c r="AG25">
         <v>0.02996866390445864</v>
       </c>
-      <c r="AG25">
+      <c r="AH25">
         <v>0.007825520005898867</v>
       </c>
-      <c r="AH25">
+      <c r="AI25">
         <v>0.01658739420425338</v>
       </c>
     </row>
@@ -3079,8 +3204,10 @@
           <t>rose_rrv_site_3-2</t>
         </is>
       </c>
-      <c r="B26">
-        <v>0</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C26">
         <v>0</v>
@@ -3089,29 +3216,29 @@
         <v>0</v>
       </c>
       <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>1.194988162460977</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>0.01323936970007425</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>0.003897704094953917</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
         <v>0.004501139330855815</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
       <c r="M26">
         <v>0</v>
       </c>
@@ -3140,42 +3267,45 @@
         <v>0</v>
       </c>
       <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
         <v>0.06206796680783593</v>
       </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
       <c r="X26">
         <v>0</v>
       </c>
       <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
         <v>0.008416598890362573</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
       <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
         <v>0.0422897788139894</v>
       </c>
-      <c r="AB26">
+      <c r="AC26">
         <v>0.008760308270813515</v>
       </c>
-      <c r="AC26">
-        <v>0</v>
-      </c>
       <c r="AD26">
         <v>0</v>
       </c>
       <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
         <v>0.6606670085234516</v>
       </c>
-      <c r="AF26">
+      <c r="AG26">
         <v>0.01744803876166532</v>
       </c>
-      <c r="AG26">
+      <c r="AH26">
         <v>0.005327013178959227</v>
       </c>
-      <c r="AH26">
+      <c r="AI26">
         <v>0</v>
       </c>
     </row>
@@ -3185,8 +3315,10 @@
           <t>rose_rrv_site_3-3</t>
         </is>
       </c>
-      <c r="B27">
-        <v>0</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C27">
         <v>0</v>
@@ -3195,38 +3327,38 @@
         <v>0</v>
       </c>
       <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <v>0.6289927450610485</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
       <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>0.03510717641984884</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>0.0001852474259123556</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>0.008286019991308498</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>0.001760100676752775</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
       <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
         <v>0.0006133056154986451</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>0.001908454463839074</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
       <c r="P27">
         <v>0</v>
       </c>
@@ -3255,33 +3387,36 @@
         <v>0</v>
       </c>
       <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
         <v>0.01251906480243646</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>0.02134805483161751</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>0.03016381540549189</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <v>0.01033422193356238</v>
       </c>
-      <c r="AC27">
-        <v>0</v>
-      </c>
       <c r="AD27">
         <v>0</v>
       </c>
       <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
         <v>0.6417608617543542</v>
       </c>
-      <c r="AF27">
+      <c r="AG27">
         <v>0.01726192566386489</v>
       </c>
-      <c r="AG27">
-        <v>0</v>
-      </c>
       <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
         <v>0</v>
       </c>
     </row>
@@ -3291,8 +3426,10 @@
           <t>rose_rrv_site_4-1</t>
         </is>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>rrv</t>
+        </is>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3301,77 +3438,77 @@
         <v>0</v>
       </c>
       <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
         <v>0.6976207074401893</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>0.01950407159828181</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <v>0.0002984777265618626</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>0.01083066508387268</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
         <v>0.002665930390541367</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
       <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <v>0.0003908019597627171</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>0.004224174888668174</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.003685931543764393</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>0.0002563091545441589</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>0.03411557725523941</v>
       </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
       <c r="S28">
         <v>0</v>
       </c>
       <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
         <v>0.02607949185437646</v>
       </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
       <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
         <v>0.01707429019802936</v>
       </c>
-      <c r="W28">
-        <v>0</v>
-      </c>
       <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
         <v>0.01093303049210691</v>
       </c>
-      <c r="Y28">
-        <v>0</v>
-      </c>
       <c r="Z28">
         <v>0</v>
       </c>
       <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
         <v>0.01751443498081838</v>
       </c>
-      <c r="AB28">
-        <v>0</v>
-      </c>
       <c r="AC28">
         <v>0</v>
       </c>
@@ -3379,15 +3516,18 @@
         <v>0</v>
       </c>
       <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
         <v>0.0682707880067947</v>
       </c>
-      <c r="AF28">
-        <v>0</v>
-      </c>
       <c r="AG28">
         <v>0</v>
       </c>
       <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
         <v>0</v>
       </c>
     </row>

</xml_diff>